<commit_message>
Controle de Caixa + Folha de funcionários
</commit_message>
<xml_diff>
--- a/2021/Janeiro/06-01-2021_FluxoDeCaixa.xlsx
+++ b/2021/Janeiro/06-01-2021_FluxoDeCaixa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm\Documents\GitHub\ConnectFibra\2021\Janeiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586E46B8-EF6A-458D-9C3E-1CE3A7F0A667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D67E54-F4C9-42B0-935B-4DE72CD5C071}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caixa de Amanda" sheetId="1" r:id="rId1"/>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +875,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4">
-        <v>95</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,7 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B13" s="19">
         <f>SUM('Caixa de Amanda'!B18,'Caixa de Jessica'!B19)</f>
-        <v>95</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>